<commit_message>
Added basic,staging and commit commands
</commit_message>
<xml_diff>
--- a/NotesGit.xlsx
+++ b/NotesGit.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Git Commands" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -15,10 +15,112 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Git Basic Commands</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>git init</t>
+  </si>
+  <si>
+    <t>initializes git reposatory.</t>
+  </si>
+  <si>
+    <t>Note: All commands to be used by launching git bash and nevigating to repo that is to be tracked</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>adds file specified to staging area</t>
+  </si>
+  <si>
+    <t>Shows status of each file in repo. 
+A File can be untracked file, in a staging area or committed file</t>
+  </si>
+  <si>
+    <t>git rm --cached &lt;file&gt;</t>
+  </si>
+  <si>
+    <t>git add &lt;File&gt;</t>
+  </si>
+  <si>
+    <t>Removes specified file from staging area</t>
+  </si>
+  <si>
+    <t>git rm --cached notes.txt</t>
+  </si>
+  <si>
+    <t>git add notes.txt</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t>Adds all modified  files into staging area</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Creating Repo</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>Staging</t>
+  </si>
+  <si>
+    <t>git commit -m "&lt; commit hint &gt; "</t>
+  </si>
+  <si>
+    <t>Commits files to git repo. Accepts commit
+ hint/Description for each commit for easy identification of changes.</t>
+  </si>
+  <si>
+    <t>git commit -m " added author info "</t>
+  </si>
+  <si>
+    <t>git log</t>
+  </si>
+  <si>
+    <t>shows log of all commits made earlier</t>
+  </si>
+  <si>
+    <t>git log --oneline</t>
+  </si>
+  <si>
+    <t>shows commit logs in single line format</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,14 +148,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +457,182 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Undo related commands
</commit_message>
<xml_diff>
--- a/NotesGit.xlsx
+++ b/NotesGit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Command</t>
   </si>
@@ -67,9 +67,6 @@
     <t>git add .</t>
   </si>
   <si>
-    <t>Adds all modified  files into staging area</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
@@ -105,6 +102,75 @@
   </si>
   <si>
     <t>shows commit logs in single line format</t>
+  </si>
+  <si>
+    <t>git checkout &lt; commit ID/ name&gt;</t>
+  </si>
+  <si>
+    <t>git checkout 4a8a0c0
+git checkout master</t>
+  </si>
+  <si>
+    <t>checks out files at specified commit as is. 
+When master is specified latest commit from master branch are checked out.</t>
+  </si>
+  <si>
+    <t>git revert &lt;commit ID&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Undo changes made in specified commit.
+ After entering command input </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:wq </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to complete execution of command</t>
+    </r>
+  </si>
+  <si>
+    <t>git revert 4a8a0c0</t>
+  </si>
+  <si>
+    <t>git reset &lt;commit ID&gt;</t>
+  </si>
+  <si>
+    <t>removes all commits above specified commit ID</t>
+  </si>
+  <si>
+    <t>git reset 4a8a0c0</t>
+  </si>
+  <si>
+    <t>git reset &lt;commit ID&gt; --hard</t>
+  </si>
+  <si>
+    <t>similar to reset command, --hard flag here premanantly deletes changes about specified commit</t>
+  </si>
+  <si>
+    <t>git reset 4a8a0c0 --hard</t>
+  </si>
+  <si>
+    <t>Undoing</t>
+  </si>
+  <si>
+    <t>Adds all modified  files into staging area. 
+Note the dot followed by add is required as part of command.</t>
   </si>
 </sst>
 </file>
@@ -136,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -144,18 +210,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,10 +545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +557,7 @@
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -483,129 +571,185 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
+      <c r="D13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added branching merging and push commands
</commit_message>
<xml_diff>
--- a/NotesGit.xlsx
+++ b/NotesGit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>Command</t>
   </si>
@@ -171,6 +171,78 @@
   <si>
     <t>Adds all modified  files into staging area. 
 Note the dot followed by add is required as part of command.</t>
+  </si>
+  <si>
+    <t>Branching</t>
+  </si>
+  <si>
+    <t>git branch &lt;Branch Name&gt;</t>
+  </si>
+  <si>
+    <t>Creates new branch with specified name</t>
+  </si>
+  <si>
+    <t>git branch feature-1</t>
+  </si>
+  <si>
+    <t>git branch -a</t>
+  </si>
+  <si>
+    <t>lists all available branches, * indicates currently pointed branch</t>
+  </si>
+  <si>
+    <t>git branch -D &lt;Branch Name&gt;</t>
+  </si>
+  <si>
+    <t>Deletes given branch. Use capital D when branch is not merged to master.</t>
+  </si>
+  <si>
+    <t>git branch -D feature-1</t>
+  </si>
+  <si>
+    <t>git checkout -b &lt;Branch Name&gt;</t>
+  </si>
+  <si>
+    <t>Creates new branch with specified name and checks it out</t>
+  </si>
+  <si>
+    <t>git checkout -b feature-a</t>
+  </si>
+  <si>
+    <t>git merge &lt;Branch Name&gt;</t>
+  </si>
+  <si>
+    <t>git merge feature-a</t>
+  </si>
+  <si>
+    <t>Merge specified branch into current branch. To merge any branch into master branch, git should be pointing to master branch before running this command.</t>
+  </si>
+  <si>
+    <t>git push &lt; repo url&gt; &lt;Branch Name&gt;</t>
+  </si>
+  <si>
+    <t>Pushes Branch content to github repo</t>
+  </si>
+  <si>
+    <t>git push https://github.com/psevekar/TestRepo.git master</t>
+  </si>
+  <si>
+    <t>git remote add &lt;alias name&gt; &lt;repo url&gt;</t>
+  </si>
+  <si>
+    <t>sets alias name for given repo link</t>
+  </si>
+  <si>
+    <t>git remote add origin https://github.com/psevekar/TestRepo.git</t>
+  </si>
+  <si>
+    <t>Push</t>
+  </si>
+  <si>
+    <t>git remote -v</t>
+  </si>
+  <si>
+    <t>shows origin url for push and fethch</t>
   </si>
 </sst>
 </file>
@@ -229,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -242,6 +314,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -545,19 +623,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -750,6 +828,118 @@
       </c>
       <c r="E16" s="4" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>